<commit_message>
almost finished, just a little more polishing
</commit_message>
<xml_diff>
--- a/ExcelToNewExcelsCreator/Files/BaseFiles/CA001 - ReplacementFile.xlsx
+++ b/ExcelToNewExcelsCreator/Files/BaseFiles/CA001 - ReplacementFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plradbad\Desktop\C#Projekty\ExcelRodipeConfigurator_AllFiles\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plradbad\source\repos\Xniba\ExcelToNewExcelsCreator\ExcelToNewExcelsCreator\Files\BaseFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1917367-E1F3-4A11-A95D-6A1A768A59A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F44DF9-6E01-4BFE-9C8A-7F57F9F63FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Carrier No:</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>156</t>
-  </si>
-  <si>
-    <t>0002</t>
   </si>
   <si>
     <t>FF FF FF AE 54 C7</t>
@@ -832,22 +829,61 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,101 +892,62 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1276,105 +1273,105 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="92" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
+      <c r="B2" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1395,105 +1392,105 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="92" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="B3" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1507,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228AAC05-854E-44AE-83B7-D8F85303EA26}">
   <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1532,10 +1529,10 @@
       <c r="E2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="83"/>
+      <c r="G2" s="65"/>
       <c r="H2" s="33" t="s">
         <v>18</v>
       </c>
@@ -1549,10 +1546,10 @@
       <c r="E3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="90" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="91"/>
+      <c r="F3" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="75"/>
       <c r="H3" s="45" t="s">
         <v>2</v>
       </c>
@@ -1564,14 +1561,14 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="66"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="16"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67"/>
       <c r="H4" s="30" t="s">
         <v>21</v>
       </c>
@@ -1585,14 +1582,14 @@
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="9"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="88" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="89"/>
+      <c r="F5" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="71"/>
       <c r="H5" s="30" t="s">
         <v>21</v>
       </c>
@@ -1612,17 +1609,17 @@
       <c r="C6" s="11"/>
       <c r="D6" s="9"/>
       <c r="E6" s="22"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="87"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="45" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="66"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="10"/>
       <c r="E7" s="23"/>
       <c r="F7" s="42"/>
@@ -1632,12 +1629,12 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="9"/>
       <c r="E8" s="22"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="89"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="41" t="s">
         <v>2</v>
       </c>
@@ -1649,8 +1646,8 @@
       <c r="C9" s="13"/>
       <c r="D9" s="9"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="87"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="45" t="s">
         <v>2</v>
       </c>
@@ -1662,8 +1659,8 @@
       <c r="C10" s="13"/>
       <c r="D10" s="9"/>
       <c r="E10" s="22"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="87"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="45" t="s">
         <v>2</v>
       </c>
@@ -1690,8 +1687,8 @@
       <c r="C12" s="13"/>
       <c r="D12" s="9"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="87"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="46" t="s">
         <v>2</v>
       </c>
@@ -1718,105 +1715,105 @@
       <c r="C14" s="13"/>
       <c r="D14" s="9"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="87"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="66"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="15"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="71"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="8"/>
       <c r="E16" s="25"/>
-      <c r="F16" s="53" t="str">
+      <c r="F16" s="83" t="str">
         <f>_xlfn.TEXTJOIN(,,MID(F5,11,1),MID(F5,13,2),MID(F5,16,2))</f>
         <v>E54C7</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="65"/>
-      <c r="C17" s="66"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="2"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
       <c r="H17" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="14"/>
       <c r="E18" s="26"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="71"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="77"/>
       <c r="H18" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="65"/>
-      <c r="C19" s="69"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="6"/>
       <c r="E19" s="27"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="64"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="92"/>
       <c r="H19" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="65"/>
-      <c r="C20" s="68"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="7"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="73"/>
       <c r="H20" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="67"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="6"/>
       <c r="E21" s="27"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="62"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="90"/>
       <c r="H21" s="45" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="65"/>
-      <c r="C22" s="68"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="2"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="58"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="88"/>
       <c r="H22" s="45" t="s">
         <v>2</v>
       </c>
@@ -1826,10 +1823,10 @@
       <c r="C23" s="48"/>
       <c r="D23" s="10"/>
       <c r="E23" s="51"/>
-      <c r="F23" s="55" t="s">
+      <c r="F23" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="56"/>
+      <c r="G23" s="86"/>
       <c r="H23" s="52" t="s">
         <v>2</v>
       </c>
@@ -1838,12 +1835,12 @@
       <c r="B24" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="72"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="76" t="s">
+      <c r="E24" s="56"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="58" t="s">
         <v>2</v>
       </c>
       <c r="J24" s="1"/>
@@ -1852,12 +1849,12 @@
       <c r="B25" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="73"/>
+      <c r="C25" s="55"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="77"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="59"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="47"/>
@@ -1875,6 +1872,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="H24:H25"/>
@@ -1891,23 +1905,6 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
@@ -1916,20 +1913,10 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="95bc305a-b46b-4a41-8e4f-996452a10042" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E370590E8A991148B057944F0E71E0E4" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0189316d4dab243999539916e0e251d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b73abb48-2cb5-4f86-8d0e-259086911774" xmlns:ns3="2541b8c9-4e93-404e-a65a-67f24201939f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4d4baf5847b53843abae870aeaced96" ns2:_="" ns3:_="">
     <xsd:import namespace="b73abb48-2cb5-4f86-8d0e-259086911774"/>
@@ -2094,37 +2081,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="95bc305a-b46b-4a41-8e4f-996452a10042" ContentTypeId="0x0101" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E7A833A-9C71-4746-ACE1-519F8CEA978F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28BE4684-EE32-4400-90F4-733F6A894CCF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BC919FB-EBEA-4A1B-8F59-58759A332712}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="2541b8c9-4e93-404e-a65a-67f24201939f"/>
-    <ds:schemaRef ds:uri="b73abb48-2cb5-4f86-8d0e-259086911774"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{134B7CF1-6ED8-4679-BB4D-96FCCB308C4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2143,10 +2123,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BC919FB-EBEA-4A1B-8F59-58759A332712}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2541b8c9-4e93-404e-a65a-67f24201939f"/>
+    <ds:schemaRef ds:uri="b73abb48-2cb5-4f86-8d0e-259086911774"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28BE4684-EE32-4400-90F4-733F6A894CCF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E7A833A-9C71-4746-ACE1-519F8CEA978F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>